<commit_message>
first pushing to github
</commit_message>
<xml_diff>
--- a/data/templates/шаблон отчета за период.xlsx
+++ b/data/templates/шаблон отчета за период.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\Days2_github\data\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{762D91EE-4CF0-4CC4-BA1C-98912C39B815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="30" windowWidth="14805" windowHeight="10500"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
@@ -13,7 +19,15 @@
     <definedName name="MyNameIs10460" localSheetId="0">'Page 1'!$A$1:$E$11</definedName>
     <definedName name="MyNameIs6367" localSheetId="0">'Page 1'!$A$1:$D$12</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -53,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -239,6 +253,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -259,17 +279,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="1"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -344,6 +358,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -604,14 +621,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -640,7 +657,7 @@
       <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -650,7 +667,7 @@
       <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="12" t="s">
         <v>9</v>
       </c>
@@ -658,7 +675,7 @@
       <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
@@ -666,7 +683,7 @@
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
@@ -674,8 +691,8 @@
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -684,16 +701,16 @@
       <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="7" t="s">
         <v>0</v>
       </c>
@@ -703,36 +720,36 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="19">
+      <c r="C9" s="17"/>
+      <c r="D9" s="21">
         <f>D2+D3+D4+D5</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="20"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="22"/>
     </row>
     <row r="11" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:4" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="str">
+      <c r="A12" s="14" t="str">
         <f ca="1">CONCATENATE("Дата построения отчета: ",TEXT(TODAY(), "ДД ММММ ГГГГ"))</f>
-        <v>Дата построения отчета: 13 Июль 2022</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
+        <v>Дата построения отчета: 18 Декабрь 2024</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>